<commit_message>
add more example test clusters
</commit_message>
<xml_diff>
--- a/test_clusters.xlsx
+++ b/test_clusters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
   <si>
     <t>kamino</t>
   </si>
@@ -260,7 +260,40 @@
     <t>achcche</t>
   </si>
   <si>
-    <t>guzarta</t>
+    <t>zarurat</t>
+  </si>
+  <si>
+    <t>zaruratmand</t>
+  </si>
+  <si>
+    <t>jatila</t>
+  </si>
+  <si>
+    <t>jatilata</t>
+  </si>
+  <si>
+    <t>itihas</t>
+  </si>
+  <si>
+    <t>itihasik</t>
+  </si>
+  <si>
+    <t>pravahita</t>
+  </si>
+  <si>
+    <t>pravaha</t>
+  </si>
+  <si>
+    <t>visheshta</t>
+  </si>
+  <si>
+    <t>vishesh</t>
+  </si>
+  <si>
+    <t>adhunik</t>
+  </si>
+  <si>
+    <t>adhunikata</t>
   </si>
   <si>
     <t>guzarne</t>
@@ -287,19 +320,19 @@
     <t>guzare</t>
   </si>
   <si>
+    <t>guzara</t>
+  </si>
+  <si>
+    <t>guzar</t>
+  </si>
+  <si>
+    <t>goojarna</t>
+  </si>
+  <si>
     <t>guzarate</t>
   </si>
   <si>
     <t>guzarata</t>
-  </si>
-  <si>
-    <t>guzara</t>
-  </si>
-  <si>
-    <t>guzar</t>
-  </si>
-  <si>
-    <t>goojarna</t>
   </si>
 </sst>
 </file>
@@ -400,10 +433,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B28" activeCellId="0" pane="topLeft" sqref="B28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A28" view="normal" windowProtection="false" workbookViewId="0" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100">
+      <selection activeCell="A35" activeCellId="0" pane="topLeft" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -734,44 +767,91 @@
       <c r="B29" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="B30" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="0" t="s">
+      <c r="B31" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="G29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+      <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+      <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L29" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="M29" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="N29" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+      <c r="A35" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="O29" s="0" t="s">
+      <c r="B35" s="0" t="s">
         <v>94</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+      <c r="A36" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>